<commit_message>
1. increase the wire width 2. merge the two brd file 3. change the fuse value and connector order 4. approve the DRC error
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="1160" yWindow="4380" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Table 1</t>
   </si>
@@ -120,6 +120,9 @@
     <t>Sabre 43160</t>
   </si>
   <si>
+    <t>Cgrid 0553</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <u/>
@@ -127,11 +130,11 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>http://www.molex.com/molex/products/datasheet.jsp?part=active/0431601102_PCB_HEADERS.xml</t>
+      <t>http://www.digikey.com/product-search/en?mpart=0705530001&amp;vendor=900</t>
     </r>
   </si>
   <si>
-    <t>Cgrid 0553</t>
+    <t>Mini FIt jr 5566</t>
   </si>
   <si>
     <r>
@@ -141,11 +144,11 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>http://www.digikey.com/product-search/en?mpart=0705530001&amp;vendor=900</t>
+      <t>http://www.molex.com/molex/products/datasheet.jsp?part=active/0469990126_PCB_HEADERS.xml</t>
     </r>
   </si>
   <si>
-    <t>Mini FIt jr 5566</t>
+    <t>Fuse 2A</t>
   </si>
   <si>
     <r>
@@ -155,11 +158,11 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>http://www.molex.com/molex/products/datasheet.jsp?part=active/0469990126_PCB_HEADERS.xml</t>
+      <t>http://www.digikey.com/product-detail/en/39612000440/WK4457BK-ND/245408</t>
     </r>
   </si>
   <si>
-    <t>Fuse 3A</t>
+    <t>Fuse 4A</t>
   </si>
   <si>
     <r>
@@ -169,11 +172,11 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>http://www.digikey.com/product-detail/en/39213150000/F5504CT-ND/3306894</t>
+      <t>http://www.digikey.com/product-detail/en/39214000000/F5505CT-ND/3306895</t>
     </r>
   </si>
   <si>
-    <t>Fuse 2A</t>
+    <t>Fuse 5A</t>
   </si>
   <si>
     <r>
@@ -183,11 +186,11 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>http://www.digikey.com/product-detail/en/39612000440/WK4457BK-ND/245408</t>
+      <t>http://www.digikey.com/product-detail/en/39615000000/WK6280CT-ND/3307368</t>
     </r>
   </si>
   <si>
-    <t>Fuse 4A</t>
+    <t>Fuse 15a</t>
   </si>
   <si>
     <r>
@@ -197,11 +200,11 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>http://www.digikey.com/product-detail/en/39214000000/F5505CT-ND/3306895</t>
+      <t>http://www.littelfuse.com/products/fuses/cartridge-fuses/5x20mm-fuses/215/215015.aspx</t>
     </r>
   </si>
   <si>
-    <t>Fuse 5A</t>
+    <t>Fuse 15a holder</t>
   </si>
   <si>
     <r>
@@ -211,11 +214,11 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>http://www.digikey.com/product-detail/en/39615000000/WK6280CT-ND/3307368</t>
+      <t>http://www.digikey.com/product-detail/en/65600001009/WK6245-ND/653441</t>
     </r>
   </si>
   <si>
-    <t>Fuse 15a</t>
+    <t xml:space="preserve">LED </t>
   </si>
   <si>
     <r>
@@ -225,11 +228,11 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>http://www.littelfuse.com/products/fuses/cartridge-fuses/5x20mm-fuses/215/215015.aspx</t>
+      <t>http://www.digikey.com/product-detail/en/LTW-2S3D8/160-1850-ND/2666499</t>
     </r>
   </si>
   <si>
-    <t>Fuse 15a holder</t>
+    <t>r1206 250</t>
   </si>
   <si>
     <r>
@@ -239,11 +242,11 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>http://www.digikey.com/product-detail/en/65600001009/WK6245-ND/653441</t>
+      <t>http://www.digikey.com/product-detail/en/Y1630250R000T9R/Y1630-250BCT-ND/4340638</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">LED </t>
+    <t>r1206 1200</t>
   </si>
   <si>
     <r>
@@ -253,11 +256,14 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>http://www.digikey.com/product-detail/en/LTW-2S3D8/160-1850-ND/2666499</t>
+      <t>http://www.digikey.com/product-detail/en/ERJ-8GEYJ122V/P1.2KECT-ND/203260</t>
     </r>
   </si>
   <si>
-    <t>r1206 250</t>
+    <t>Following is Not on board</t>
+  </si>
+  <si>
+    <t>Cgrid - plug</t>
   </si>
   <si>
     <r>
@@ -267,11 +273,11 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>http://www.digikey.com/product-detail/en/Y1630250R000T9R/Y1630-250BCT-ND/4340638</t>
+      <t>http://www.digikey.com/product-detail/en/0050579202/WM5363-ND/2731427</t>
     </r>
   </si>
   <si>
-    <t>r1206 1200</t>
+    <t>Fit jr - plug</t>
   </si>
   <si>
     <r>
@@ -281,14 +287,11 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>http://www.digikey.com/product-detail/en/ERJ-8GEYJ122V/P1.2KECT-ND/203260</t>
+      <t>http://www.molex.com/molex/products/datasheet.jsp?part=active/0039012020_CRIMP_HOUSINGS.xml</t>
     </r>
   </si>
   <si>
-    <t>Following is Not on board</t>
-  </si>
-  <si>
-    <t>Cgrid - plug</t>
+    <t>Sabre - plug</t>
   </si>
   <si>
     <r>
@@ -298,11 +301,14 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>http://www.digikey.com/product-detail/en/0050579202/WM5363-ND/2731427</t>
+      <t>http://www.molex.com/molex/products/datasheet.jsp?part=active/0444411002_CRIMP_HOUSINGS.xml</t>
     </r>
   </si>
   <si>
-    <t>Fit jr - plug</t>
+    <t xml:space="preserve">heat sink </t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/7-340-2PP-BA/294-1080-ND/272718</t>
   </si>
   <si>
     <r>
@@ -312,28 +318,9 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>http://www.molex.com/molex/products/datasheet.jsp?part=active/0039012020_CRIMP_HOUSINGS.xml</t>
+      <t>http://www.molex.com/molex/products/datasheet.jsp?part=active/0431601102_PCB_HEADERS.xml</t>
     </r>
-  </si>
-  <si>
-    <t>Sabre - plug</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>http://www.molex.com/molex/products/datasheet.jsp?part=active/0444411002_CRIMP_HOUSINGS.xml</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">heat sink </t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/7-340-2PP-BA/294-1080-ND/272718</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -489,16 +476,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1823,13 +1810,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV25"/>
+  <dimension ref="A1:IV24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -1841,17 +1828,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="20.5" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -1980,7 +1967,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -1991,13 +1978,13 @@
     </row>
     <row r="10" spans="1:9" ht="20.25" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="4">
         <v>5</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -2008,13 +1995,13 @@
     </row>
     <row r="11" spans="1:9" ht="18.5" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="4">
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -2025,13 +2012,13 @@
     </row>
     <row r="12" spans="1:9" ht="20.25" customHeight="1">
       <c r="A12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4">
+        <v>8</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="B12" s="4">
-        <v>2</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -2042,13 +2029,13 @@
     </row>
     <row r="13" spans="1:9" ht="20.25" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4">
         <v>4</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -2059,13 +2046,13 @@
     </row>
     <row r="14" spans="1:9" ht="20.25" customHeight="1">
       <c r="A14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -2076,13 +2063,13 @@
     </row>
     <row r="15" spans="1:9" ht="20.25" customHeight="1">
       <c r="A15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="4">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B15" s="4">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -2093,13 +2080,13 @@
     </row>
     <row r="16" spans="1:9" ht="20.25" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -2110,13 +2097,13 @@
     </row>
     <row r="17" spans="1:9" ht="20.25" customHeight="1">
       <c r="A17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="4">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="B17" s="4">
-        <v>1</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -2127,13 +2114,13 @@
     </row>
     <row r="18" spans="1:9" ht="20.25" customHeight="1">
       <c r="A18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="4">
-        <v>2</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -2144,13 +2131,13 @@
     </row>
     <row r="19" spans="1:9" ht="20.25" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -2160,14 +2147,14 @@
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="4">
+      <c r="A20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="8">
         <v>1</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>39</v>
+      <c r="C20" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -2176,16 +2163,12 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A21" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="10">
-        <v>1</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>48</v>
-      </c>
+    <row r="21" spans="1:9" ht="32.25" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -2193,12 +2176,16 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9" ht="32.25" customHeight="1">
+    <row r="22" spans="1:9" ht="20.25" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="B22" s="4">
+        <v>5</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -2208,13 +2195,13 @@
     </row>
     <row r="23" spans="1:9" ht="20.25" customHeight="1">
       <c r="A23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="4">
+        <v>6</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="B23" s="4">
-        <v>5</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -2225,37 +2212,20 @@
     </row>
     <row r="24" spans="1:9" ht="20.25" customHeight="1">
       <c r="A24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="4">
-        <v>6</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A25" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="4">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2280,10 +2250,9 @@
     <hyperlink ref="C17" r:id="rId15"/>
     <hyperlink ref="C18" r:id="rId16"/>
     <hyperlink ref="C19" r:id="rId17"/>
-    <hyperlink ref="C20" r:id="rId18"/>
+    <hyperlink ref="C22" r:id="rId18"/>
     <hyperlink ref="C23" r:id="rId19"/>
     <hyperlink ref="C24" r:id="rId20"/>
-    <hyperlink ref="C25" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>